<commit_message>
checkout stripe finished, admin dashbord
</commit_message>
<xml_diff>
--- a/app/data/products.xlsx
+++ b/app/data/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tradirest-my.sharepoint.com/personal/riegallieni_empreintes_paris/Documents/Bureau/dev/end_bootcamp_exo/Concreate/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{1C21E7FB-F33D-466E-B935-0AC2FE52B5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7939720-39B0-49B3-9875-9A6CF80B39C2}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{880600E9-76B1-44E0-8C5E-088321C41745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1ADB5852-7879-441A-ACB2-4B637EA60FB4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{476E44CA-D021-4E9C-A5CE-94A2DE88963E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>Two-piece reversible layout;Monolithic concrete volume;Chamfered facets for sharp light;Micro-texture sealed top;Anti-slip pads + levelers</t>
+  </si>
+  <si>
+    <t>Raw lamp</t>
+  </si>
+  <si>
+    <t>Brutalist pure lamp.</t>
+  </si>
+  <si>
+    <t>CC-FA-260212-01</t>
+  </si>
+  <si>
+    <t>assets/products/prod_3_1.png;assets/products/prod_3_2.png;assets/products/prod_3_3.png;assets/products/prod_3_4.png</t>
   </si>
 </sst>
 </file>
@@ -451,10 +463,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CE47A9-4E97-4461-8A43-6A87A6C0342F}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,7 +539,28 @@
         <v>15</v>
       </c>
     </row>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>340</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>